<commit_message>
write common work ui
</commit_message>
<xml_diff>
--- a/public/locales/multilanguage.xlsx
+++ b/public/locales/multilanguage.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223">
   <si>
     <t>标记</t>
   </si>
@@ -145,22 +145,13 @@
     <t>请输入Dapp标签</t>
   </si>
   <si>
-    <t>dapp_name</t>
-  </si>
-  <si>
-    <t>The name of Dapp</t>
-  </si>
-  <si>
-    <t>Dapp名称</t>
-  </si>
-  <si>
-    <t>dapp_label</t>
-  </si>
-  <si>
-    <t>The label of Dapp</t>
-  </si>
-  <si>
-    <t>Dapp标签</t>
+    <t>dao_name</t>
+  </si>
+  <si>
+    <t>The name of DAO</t>
+  </si>
+  <si>
+    <t>DAO名称</t>
   </si>
   <si>
     <t>reset</t>
@@ -172,31 +163,22 @@
     <t>清空重来</t>
   </si>
   <si>
-    <t>dapp_address</t>
-  </si>
-  <si>
-    <t>The address of Dapp</t>
-  </si>
-  <si>
-    <t>Dapp地址</t>
+    <t>dao_address</t>
+  </si>
+  <si>
+    <t>The address of DAO</t>
+  </si>
+  <si>
+    <t>DAO地址</t>
   </si>
   <si>
     <t>creator</t>
   </si>
   <si>
-    <t>The address of manager</t>
-  </si>
-  <si>
-    <t>管理员地址</t>
-  </si>
-  <si>
-    <t>dapp_id</t>
-  </si>
-  <si>
-    <t>The id of Dapp</t>
-  </si>
-  <si>
-    <t>Dapp编号</t>
+    <t>The address of Creator</t>
+  </si>
+  <si>
+    <t>创建者地址</t>
   </si>
   <si>
     <t>create_time</t>
@@ -208,76 +190,67 @@
     <t>注册时间</t>
   </si>
   <si>
-    <t>dapp_description</t>
-  </si>
-  <si>
-    <t>The description of Dapp</t>
-  </si>
-  <si>
-    <t>Dapp简介</t>
-  </si>
-  <si>
-    <t>dapp_website</t>
-  </si>
-  <si>
-    <t>The website of Dapp</t>
-  </si>
-  <si>
-    <t>Dapp主页</t>
-  </si>
-  <si>
-    <t>full_dapp</t>
-  </si>
-  <si>
-    <t>The detail of Dapp</t>
-  </si>
-  <si>
-    <t>Dapp详情</t>
-  </si>
-  <si>
-    <t>latest_dapp</t>
-  </si>
-  <si>
-    <t>The Latest Dapps</t>
-  </si>
-  <si>
-    <t>最新Dapp</t>
-  </si>
-  <si>
-    <t>dapp_amount</t>
-  </si>
-  <si>
-    <t>Has {amount} Dapps</t>
-  </si>
-  <si>
-    <t>共有{amount} 个Dapp</t>
-  </si>
-  <si>
-    <t>show_dapp</t>
-  </si>
-  <si>
-    <t>Click name to entry the detail </t>
-  </si>
-  <si>
-    <t>点击标题可以跳转到详情</t>
-  </si>
-  <si>
-    <t>no_dapp</t>
-  </si>
-  <si>
-    <t>Current dapp does not exist</t>
-  </si>
-  <si>
-    <t>当前Dapp不存在</t>
-  </si>
-  <si>
-    <t>search_dapp_first</t>
-  </si>
-  <si>
-    <t>Please search the dapp first</t>
-  </si>
-  <si>
-    <t>请先查询Dapp</t>
+    <t>dao_description</t>
+  </si>
+  <si>
+    <t>The description of DAO</t>
+  </si>
+  <si>
+    <t>DAO简介</t>
+  </si>
+  <si>
+    <t>full_dao</t>
+  </si>
+  <si>
+    <t>The detail of DAO</t>
+  </si>
+  <si>
+    <t>DAO详情</t>
+  </si>
+  <si>
+    <t>latest_dao</t>
+  </si>
+  <si>
+    <t>The Latest DAOS</t>
+  </si>
+  <si>
+    <t>最新DAO</t>
+  </si>
+  <si>
+    <t>dao_amount</t>
+  </si>
+  <si>
+    <t>Has {amount} DAOS</t>
+  </si>
+  <si>
+    <t>共有{amount} 个DAO</t>
+  </si>
+  <si>
+    <t>show_dao</t>
+  </si>
+  <si>
+    <t>Click address to entry the detail </t>
+  </si>
+  <si>
+    <t>点击地址可以跳转到详情</t>
+  </si>
+  <si>
+    <t>no_dao</t>
+  </si>
+  <si>
+    <t>Current DAO does not exist</t>
+  </si>
+  <si>
+    <t>当前DAO不存在</t>
+  </si>
+  <si>
+    <t>search_dao_first</t>
+  </si>
+  <si>
+    <t>Please search the DAO first</t>
+  </si>
+  <si>
+    <t>请先查询DAO</t>
   </si>
   <si>
     <t>dapp_method_list</t>
@@ -361,6 +334,177 @@
     <t>参数示例</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>名称</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>地址</t>
+  </si>
+  <si>
+    <t>owner_amount</t>
+  </si>
+  <si>
+    <t>Has {amount} owners</t>
+  </si>
+  <si>
+    <t>共有{amount} 个管理员</t>
+  </si>
+  <si>
+    <t>owner_admin</t>
+  </si>
+  <si>
+    <t>Admin owners</t>
+  </si>
+  <si>
+    <t>管理员管理</t>
+  </si>
+  <si>
+    <t>owner_address_i</t>
+  </si>
+  <si>
+    <t>The address of owner[{amount}]</t>
+  </si>
+  <si>
+    <t>管理员地址[{amount}]</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>移除</t>
+  </si>
+  <si>
+    <t>replace</t>
+  </si>
+  <si>
+    <t>Replace</t>
+  </si>
+  <si>
+    <t>替换</t>
+  </si>
+  <si>
+    <t>add_owner</t>
+  </si>
+  <si>
+    <t>Add a owner</t>
+  </si>
+  <si>
+    <t>增加管理员</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>增加</t>
+  </si>
+  <si>
+    <t>input_new_owner</t>
+  </si>
+  <si>
+    <t>Input the address of new owner</t>
+  </si>
+  <si>
+    <t>请输入新管理员地址</t>
+  </si>
+  <si>
+    <t>null_input</t>
+  </si>
+  <si>
+    <t>Null input</t>
+  </si>
+  <si>
+    <t>输入不能为空</t>
+  </si>
+  <si>
+    <t>zero_address</t>
+  </si>
+  <si>
+    <t>Address is zero address</t>
+  </si>
+  <si>
+    <t>输入不能为零地址</t>
+  </si>
+  <si>
+    <t>invalid_address</t>
+  </si>
+  <si>
+    <t>Address is invalid</t>
+  </si>
+  <si>
+    <t>输入地址格式错误</t>
+  </si>
+  <si>
+    <t>owner_existed</t>
+  </si>
+  <si>
+    <t>The owner address has existed</t>
+  </si>
+  <si>
+    <t>管理员已经存在</t>
+  </si>
+  <si>
+    <t>replace_owner</t>
+  </si>
+  <si>
+    <t>Replace Owner</t>
+  </si>
+  <si>
+    <t>替换管理员</t>
+  </si>
+  <si>
+    <t>replace_address</t>
+  </si>
+  <si>
+    <t>Replace the owner of address {address}</t>
+  </si>
+  <si>
+    <t>替换地址为{address}的管理员</t>
+  </si>
+  <si>
+    <t>new_owner_address</t>
+  </si>
+  <si>
+    <t>New Owner Address</t>
+  </si>
+  <si>
+    <t>新管理员地址</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>取消</t>
+  </si>
+  <si>
+    <t>confirm</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>确认</t>
+  </si>
+  <si>
     <t>guide</t>
   </si>
   <si>
@@ -406,13 +550,13 @@
     <t>无</t>
   </si>
   <si>
-    <t>full_article</t>
-  </si>
-  <si>
-    <t>Full Content</t>
-  </si>
-  <si>
-    <t>文章全文</t>
+    <t>transfer_eth_admin</t>
+  </si>
+  <si>
+    <t>Transfer ETH out</t>
+  </si>
+  <si>
+    <t>ETH转出</t>
   </si>
   <si>
     <t>url_copied</t>
@@ -433,145 +577,112 @@
     <t>点击分享</t>
   </si>
   <si>
-    <t>deme</t>
-  </si>
-  <si>
-    <t>DeMe</t>
-  </si>
-  <si>
-    <t>去中心化媒体</t>
-  </si>
-  <si>
-    <t>reward_author</t>
-  </si>
-  <si>
-    <t>Reward author</t>
-  </si>
-  <si>
-    <t>打赏作者</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>https://naturaldao.io/tool/editor.html</t>
-  </si>
-  <si>
-    <t>https://naturaldao.io/cn/tool-2/editor.html</t>
-  </si>
-  <si>
-    <t>editor</t>
-  </si>
-  <si>
-    <t>Editor</t>
-  </si>
-  <si>
-    <t>编辑器</t>
-  </si>
-  <si>
-    <t>dmn</t>
-  </si>
-  <si>
-    <t>Decentralized Media Network</t>
-  </si>
-  <si>
-    <t>去中心化媒体网络</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>register_a_name</t>
-  </si>
-  <si>
-    <t>Register a name</t>
-  </si>
-  <si>
-    <t>注册昵称</t>
-  </si>
-  <si>
-    <t>new_name</t>
-  </si>
-  <si>
-    <t>New name</t>
-  </si>
-  <si>
-    <t>新昵称</t>
-  </si>
-  <si>
-    <t>hasUpload</t>
-  </si>
-  <si>
-    <t>Uploaded</t>
-  </si>
-  <si>
-    <t>已上传</t>
-  </si>
-  <si>
-    <t>public</t>
-  </si>
-  <si>
-    <t>Public</t>
-  </si>
-  <si>
-    <t>公共</t>
-  </si>
-  <si>
-    <t>private</t>
-  </si>
-  <si>
-    <t>Private</t>
-  </si>
-  <si>
-    <t>私有</t>
-  </si>
-  <si>
-    <t>select_svg_type</t>
-  </si>
-  <si>
-    <t>Please set the type of image</t>
-  </si>
-  <si>
-    <t>请选择图片类型</t>
-  </si>
-  <si>
-    <t>all_svg</t>
-  </si>
-  <si>
-    <t>All Images</t>
-  </si>
-  <si>
-    <t>图库</t>
-  </si>
-  <si>
-    <t>show_all_svg</t>
-  </si>
-  <si>
-    <t>Public Images</t>
-  </si>
-  <si>
-    <t>公共图片</t>
-  </si>
-  <si>
-    <t>click_to_copy</t>
-  </si>
-  <si>
-    <t>Copy</t>
-  </si>
-  <si>
-    <t>复制</t>
-  </si>
-  <si>
-    <t>code_copied</t>
-  </si>
-  <si>
-    <t>The source code of image has been copied</t>
-  </si>
-  <si>
-    <t>图片代码已经复制</t>
+    <t>recipient</t>
+  </si>
+  <si>
+    <t>Recipient</t>
+  </si>
+  <si>
+    <t>接收地址</t>
+  </si>
+  <si>
+    <t>input_transfer_value</t>
+  </si>
+  <si>
+    <t>Input amount of ether</t>
+  </si>
+  <si>
+    <t>输入ETH数量</t>
+  </si>
+  <si>
+    <t>eth_amount</t>
+  </si>
+  <si>
+    <t>The balance of DAO</t>
+  </si>
+  <si>
+    <t>DAO账号余额</t>
+  </si>
+  <si>
+    <t>transfer_value</t>
+  </si>
+  <si>
+    <t>Amount of ethers</t>
+  </si>
+  <si>
+    <t>ETH数量</t>
+  </si>
+  <si>
+    <t>transfer_out</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>转出</t>
+  </si>
+  <si>
+    <t>invalid_number</t>
+  </si>
+  <si>
+    <t>Invalid amount of ether</t>
+  </si>
+  <si>
+    <t>请输入正确的ETH数量</t>
+  </si>
+  <si>
+    <t>custom_work</t>
+  </si>
+  <si>
+    <t>Custom Work</t>
+  </si>
+  <si>
+    <t>一般事务</t>
+  </si>
+  <si>
+    <t>call_address</t>
+  </si>
+  <si>
+    <t>Contract Address</t>
+  </si>
+  <si>
+    <t>调用合约地址</t>
+  </si>
+  <si>
+    <t>call_value</t>
+  </si>
+  <si>
+    <t>Amount of ether to pay</t>
+  </si>
+  <si>
+    <t>发送的ETH数量</t>
+  </si>
+  <si>
+    <t>call_data</t>
+  </si>
+  <si>
+    <t>encoded call data</t>
+  </si>
+  <si>
+    <t>编码后的调用数据</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>提交</t>
+  </si>
+  <si>
+    <t>invalid_call_data</t>
+  </si>
+  <si>
+    <t>Invalid encoded call data</t>
+  </si>
+  <si>
+    <t>无效的编码数据</t>
   </si>
 </sst>
 </file>
@@ -579,12 +690,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -599,13 +710,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF70B1E7"/>
       <name val="宋体"/>
@@ -614,9 +718,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -627,8 +737,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -649,18 +766,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -672,8 +790,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -696,8 +822,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -710,40 +837,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -757,12 +852,20 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -779,6 +882,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -791,169 +924,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -970,8 +1073,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -979,8 +1082,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -995,21 +1107,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1030,17 +1127,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1056,11 +1153,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1069,152 +1172,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1236,16 +1339,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1567,10 +1664,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5" defaultRowHeight="17.6" outlineLevelCol="2"/>
@@ -1838,7 +1935,7 @@
       <c r="A24" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -1849,7 +1946,7 @@
       <c r="A25" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -1871,7 +1968,7 @@
       <c r="A27" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -1882,7 +1979,7 @@
       <c r="A28" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -1951,7 +2048,7 @@
       <c r="B34" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1984,7 +2081,7 @@
       <c r="B37" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2010,311 +2107,403 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="7"/>
-    </row>
-    <row r="41" spans="2:3">
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-    </row>
-    <row r="45" spans="2:3">
-      <c r="B45" s="7"/>
-      <c r="C45" s="8"/>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="7"/>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="7"/>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="7"/>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="7"/>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="7"/>
-    </row>
-    <row r="54" spans="2:2">
-      <c r="B54" s="7"/>
-    </row>
-    <row r="55" spans="2:2">
-      <c r="B55" s="7"/>
+    <row r="40" ht="18" spans="1:3">
+      <c r="A40" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" ht="18" spans="1:3">
+      <c r="A41" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" ht="18" spans="1:3">
+      <c r="A42" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" ht="18" spans="1:3">
+      <c r="A43" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" ht="18" spans="1:3">
+      <c r="A44" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" ht="18" spans="1:3">
+      <c r="A45" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" ht="18" spans="1:3">
+      <c r="A46" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="47" ht="18" spans="1:3">
+      <c r="A47" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" ht="18" spans="1:3">
+      <c r="A48" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" ht="18" spans="1:3">
+      <c r="A49" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" ht="18" spans="1:3">
+      <c r="A50" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" ht="18" spans="1:3">
+      <c r="A51" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" ht="18" spans="1:3">
+      <c r="A52" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" ht="18" spans="1:3">
+      <c r="A53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" ht="18" spans="1:3">
+      <c r="A54" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" ht="18" spans="1:3">
+      <c r="A55" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" ht="18" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" ht="18" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" ht="18" spans="1:3">
+      <c r="A58" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="59" ht="18" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>115</v>
+        <v>172</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>116</v>
+        <v>173</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>117</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" ht="18" spans="1:3">
       <c r="A60" s="1" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>120</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" ht="18" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>123</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" ht="18" spans="1:3">
       <c r="A62" s="1" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>126</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" ht="18" spans="1:3">
       <c r="A63" s="1" t="s">
-        <v>127</v>
+        <v>184</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>128</v>
+        <v>185</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" ht="18" spans="1:3">
       <c r="A64" s="1" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>131</v>
+        <v>188</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>132</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" ht="18" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="66" ht="18" spans="1:3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>138</v>
+        <v>193</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="67" ht="18" spans="1:3">
       <c r="A67" s="1" t="s">
-        <v>139</v>
+        <v>196</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>140</v>
+        <v>197</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="68" ht="18" spans="1:3">
-      <c r="A68" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="69" ht="18" spans="1:3">
       <c r="A69" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>147</v>
+        <v>202</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="70" ht="18" spans="1:3">
       <c r="A70" s="1" t="s">
-        <v>148</v>
+        <v>205</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>149</v>
+        <v>206</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="71" ht="18" spans="1:3">
       <c r="A71" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>153</v>
+        <v>208</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="72" ht="18" spans="1:3">
       <c r="A72" s="1" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>2</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73" ht="18" spans="1:3">
       <c r="A73" s="1" t="s">
-        <v>156</v>
+        <v>214</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>157</v>
+        <v>215</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>158</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" ht="18" spans="1:3">
       <c r="A74" s="1" t="s">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>160</v>
+        <v>218</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>161</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" ht="18" spans="1:3">
       <c r="A75" s="1" t="s">
-        <v>162</v>
+        <v>220</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>163</v>
+        <v>221</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="76" ht="18" spans="1:3">
-      <c r="A76" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="77" ht="18" spans="1:3">
-      <c r="A77" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="78" ht="18" spans="1:3">
-      <c r="A78" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="79" ht="18" spans="1:3">
-      <c r="A79" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="80" ht="18" spans="1:3">
-      <c r="A80" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="81" ht="18" spans="1:3">
-      <c r="A81" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="82" ht="18" spans="1:3">
-      <c r="A82" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>185</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B69" r:id="rId1" display="https://naturaldao.io/tool/editor.html" tooltip="https://naturaldao.io/tool/editor.html"/>
-    <hyperlink ref="C69" r:id="rId2" display="https://naturaldao.io/cn/tool-2/editor.html" tooltip="https://naturaldao.io/cn/tool-2/editor.html"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add some ui and trait
</commit_message>
<xml_diff>
--- a/public/locales/multilanguage.xlsx
+++ b/public/locales/multilanguage.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238">
   <si>
     <t>标记</t>
   </si>
@@ -367,7 +367,7 @@
     <t>Admin owners</t>
   </si>
   <si>
-    <t>管理员管理</t>
+    <t>Owner管理</t>
   </si>
   <si>
     <t>owner_address_i</t>
@@ -631,13 +631,13 @@
     <t>请输入正确的ETH数量</t>
   </si>
   <si>
-    <t>custom_work</t>
-  </si>
-  <si>
-    <t>Custom Work</t>
-  </si>
-  <si>
-    <t>一般事务</t>
+    <t>custom_transaction</t>
+  </si>
+  <si>
+    <t>Custom transaction</t>
+  </si>
+  <si>
+    <t>自定义事务</t>
   </si>
   <si>
     <t>call_address</t>
@@ -652,7 +652,7 @@
     <t>call_value</t>
   </si>
   <si>
-    <t>Amount of ether to pay</t>
+    <t>Amount of ether to transfer</t>
   </si>
   <si>
     <t>发送的ETH数量</t>
@@ -683,6 +683,51 @@
   </si>
   <si>
     <t>无效的编码数据</t>
+  </si>
+  <si>
+    <t>common_transactions</t>
+  </si>
+  <si>
+    <t>Common transactions</t>
+  </si>
+  <si>
+    <t>常用事务</t>
+  </si>
+  <si>
+    <t>select_transction</t>
+  </si>
+  <si>
+    <t>Select a transaction</t>
+  </si>
+  <si>
+    <t>选择一项事务</t>
+  </si>
+  <si>
+    <t>transfer_20_token</t>
+  </si>
+  <si>
+    <t>Transfer ERC20 tokens</t>
+  </si>
+  <si>
+    <t>转移ERC20代币</t>
+  </si>
+  <si>
+    <t>token_address</t>
+  </si>
+  <si>
+    <t>The address of token</t>
+  </si>
+  <si>
+    <t>代币合约地址</t>
+  </si>
+  <si>
+    <t>transfer_20_token_amount</t>
+  </si>
+  <si>
+    <t>Amount of tokens to transfer</t>
+  </si>
+  <si>
+    <t>转移代币数量</t>
   </si>
 </sst>
 </file>
@@ -692,10 +737,10 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -723,8 +768,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="21"/>
+      <color rgb="FF222222"/>
+      <name val="Arial Unicode MS"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -737,23 +795,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -774,17 +818,85 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -799,73 +911,12 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -876,19 +927,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,163 +1077,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1075,39 +1126,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1142,12 +1160,25 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1167,157 +1198,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1344,6 +1395,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1664,10 +1718,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5" defaultRowHeight="17.6" outlineLevelCol="2"/>
@@ -2503,6 +2557,61 @@
         <v>222</v>
       </c>
     </row>
+    <row r="76" ht="29.2" spans="1:3">
+      <c r="A76" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="77" ht="18" spans="1:3">
+      <c r="A77" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="78" ht="18" spans="1:3">
+      <c r="A78" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="79" ht="18" spans="1:3">
+      <c r="A79" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="80" ht="18" spans="1:3">
+      <c r="A80" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
seal the templateOne ui
</commit_message>
<xml_diff>
--- a/public/locales/multilanguage.xlsx
+++ b/public/locales/multilanguage.xlsx
@@ -740,7 +740,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -753,25 +753,6 @@
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF70B1E7"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="21"/>
-      <color rgb="FF222222"/>
-      <name val="Arial Unicode MS"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1223,163 +1204,154 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1390,13 +1362,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1720,8 +1686,8 @@
   <sheetPr/>
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5" defaultRowHeight="17.6" outlineLevelCol="2"/>
@@ -1733,574 +1699,574 @@
   </cols>
   <sheetData>
     <row r="1" ht="18" spans="1:3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="18" spans="1:3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" ht="18" spans="1:3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="18" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" ht="18" spans="1:3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" ht="18" spans="1:3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" ht="18" spans="1:3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" ht="18" spans="1:3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" ht="18" spans="1:3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" ht="18" spans="1:3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" ht="36" spans="1:3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" ht="18" spans="1:3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" ht="18" spans="1:3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" ht="18" spans="1:3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" ht="18" spans="1:3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" ht="18" spans="1:3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" ht="18" spans="1:3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="18" ht="18" spans="1:3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" ht="18" spans="1:3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="20" ht="18" spans="1:3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" ht="18" spans="1:3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" ht="18" spans="1:3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="23" ht="18" spans="1:3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="24" ht="18" spans="1:3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="25" ht="18" spans="1:3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="26" ht="18" spans="1:3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="27" ht="18" spans="1:3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="28" ht="18" spans="1:3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="29" ht="18" spans="1:3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="30" ht="18" spans="1:3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="31" ht="18" spans="1:3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="32" ht="18" spans="1:3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="33" ht="18" spans="1:3">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="34" ht="18" spans="1:3">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="35" ht="18" spans="1:3">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="36" ht="18" spans="1:3">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="37" ht="18" spans="1:3">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="38" ht="18" spans="1:3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="39" ht="18" spans="1:3">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="40" ht="18" spans="1:3">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="41" ht="18" spans="1:3">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="3" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="42" ht="18" spans="1:3">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="43" ht="18" spans="1:3">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="44" ht="18" spans="1:3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="45" ht="18" spans="1:3">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="46" ht="18" spans="1:3">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="47" ht="18" spans="1:3">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="3" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="48" ht="18" spans="1:3">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="49" ht="18" spans="1:3">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="50" ht="18" spans="1:3">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="3" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="51" ht="18" spans="1:3">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="3" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="52" ht="18" spans="1:3">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="3" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2451,10 +2417,10 @@
       <c r="A66" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="1" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2470,13 +2436,13 @@
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="1" t="s">
         <v>201</v>
       </c>
     </row>
@@ -2557,11 +2523,11 @@
         <v>222</v>
       </c>
     </row>
-    <row r="76" ht="29.2" spans="1:3">
+    <row r="76" ht="18" spans="1:3">
       <c r="A76" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B76" s="4" t="s">
         <v>224</v>
       </c>
       <c r="C76" s="3" t="s">

</xml_diff>